<commit_message>
Agregada división de pragmáticos en Mayoría Temprana y Tardía con filtro interactivo
</commit_message>
<xml_diff>
--- a/data/dataset_valores.xlsx
+++ b/data/dataset_valores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eriksandoval/Desktop/ZAGAZ/Estaciones/CH4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994AB10A-EFE9-B745-B2EE-49A0BB08C13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E01F3CC-1A55-554D-8918-F79D0DD6175B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="760" windowWidth="30160" windowHeight="18880" xr2:uid="{80066C9F-7D8E-B340-8F04-A05F2EBF0A6F}"/>
   </bookViews>
@@ -1478,7 +1478,7 @@
   <dimension ref="A1:X261"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J143" sqref="J143"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1999,7 +1999,7 @@
         <v>56</v>
       </c>
       <c r="W7" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X7" t="s">
         <v>58</v>
@@ -2419,7 +2419,7 @@
         <v>30</v>
       </c>
       <c r="O13" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P13" t="s">
         <v>32</v>
@@ -2739,7 +2739,7 @@
         <v>38</v>
       </c>
       <c r="W17" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X17" t="s">
         <v>40</v>
@@ -3331,7 +3331,7 @@
         <v>56</v>
       </c>
       <c r="W25" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X25" t="s">
         <v>58</v>
@@ -3455,7 +3455,7 @@
         <v>36</v>
       </c>
       <c r="O27" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P27" t="s">
         <v>46</v>
@@ -5181,7 +5181,7 @@
         <v>38</v>
       </c>
       <c r="W50" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X50" t="s">
         <v>40</v>
@@ -5625,7 +5625,7 @@
         <v>56</v>
       </c>
       <c r="W56" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X56" t="s">
         <v>40</v>
@@ -5897,7 +5897,7 @@
         <v>36</v>
       </c>
       <c r="O60" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P60" t="s">
         <v>32</v>
@@ -7451,7 +7451,7 @@
         <v>30</v>
       </c>
       <c r="O81" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P81" t="s">
         <v>46</v>
@@ -8807,7 +8807,7 @@
         <v>38</v>
       </c>
       <c r="W99" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X99" t="s">
         <v>40</v>
@@ -8881,7 +8881,7 @@
         <v>38</v>
       </c>
       <c r="W100" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X100" t="s">
         <v>40</v>
@@ -8931,7 +8931,7 @@
         <v>36</v>
       </c>
       <c r="O101" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P101" t="s">
         <v>97</v>
@@ -9005,7 +9005,7 @@
         <v>30</v>
       </c>
       <c r="O102" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P102" t="s">
         <v>46</v>
@@ -10707,7 +10707,7 @@
         <v>36</v>
       </c>
       <c r="O125" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P125" t="s">
         <v>97</v>
@@ -10781,7 +10781,7 @@
         <v>30</v>
       </c>
       <c r="O126" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P126" t="s">
         <v>67</v>
@@ -11077,7 +11077,7 @@
         <v>30</v>
       </c>
       <c r="O130" t="s">
-        <v>89</v>
+        <v>37</v>
       </c>
       <c r="P130" t="s">
         <v>32</v>
@@ -11225,7 +11225,7 @@
         <v>36</v>
       </c>
       <c r="O132" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P132" t="s">
         <v>32</v>
@@ -11471,7 +11471,7 @@
         <v>56</v>
       </c>
       <c r="W135" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X135" t="s">
         <v>58</v>
@@ -11989,7 +11989,7 @@
         <v>38</v>
       </c>
       <c r="W142" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X142" t="s">
         <v>40</v>
@@ -12039,7 +12039,7 @@
         <v>36</v>
       </c>
       <c r="O143" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P143" t="s">
         <v>32</v>
@@ -12285,7 +12285,7 @@
         <v>38</v>
       </c>
       <c r="W146" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X146" t="s">
         <v>40</v>
@@ -13223,7 +13223,7 @@
         <v>36</v>
       </c>
       <c r="O159" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P159" t="s">
         <v>46</v>
@@ -13765,7 +13765,7 @@
         <v>56</v>
       </c>
       <c r="W166" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X166" t="s">
         <v>40</v>
@@ -14037,7 +14037,7 @@
         <v>36</v>
       </c>
       <c r="O170" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P170" t="s">
         <v>98</v>
@@ -14407,7 +14407,7 @@
         <v>36</v>
       </c>
       <c r="O175" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P175" t="s">
         <v>46</v>
@@ -14727,7 +14727,7 @@
         <v>38</v>
       </c>
       <c r="W179" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X179" t="s">
         <v>40</v>
@@ -14925,7 +14925,7 @@
         <v>36</v>
       </c>
       <c r="O182" t="s">
-        <v>89</v>
+        <v>37</v>
       </c>
       <c r="P182" t="s">
         <v>46</v>
@@ -15221,7 +15221,7 @@
         <v>36</v>
       </c>
       <c r="O186" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P186" t="s">
         <v>87</v>
@@ -15615,7 +15615,7 @@
         <v>38</v>
       </c>
       <c r="W191" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X191" t="s">
         <v>40</v>
@@ -15689,7 +15689,7 @@
         <v>56</v>
       </c>
       <c r="W192" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X192" t="s">
         <v>74</v>
@@ -16479,7 +16479,7 @@
         <v>30</v>
       </c>
       <c r="O203" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P203" t="s">
         <v>98</v>
@@ -16627,7 +16627,7 @@
         <v>30</v>
       </c>
       <c r="O205" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P205" t="s">
         <v>98</v>
@@ -17071,7 +17071,7 @@
         <v>30</v>
       </c>
       <c r="O211" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P211" t="s">
         <v>32</v>
@@ -17589,7 +17589,7 @@
         <v>36</v>
       </c>
       <c r="O218" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P218" t="s">
         <v>32</v>
@@ -18033,7 +18033,7 @@
         <v>36</v>
       </c>
       <c r="O224" t="s">
-        <v>89</v>
+        <v>37</v>
       </c>
       <c r="P224" t="s">
         <v>32</v>
@@ -18995,7 +18995,7 @@
         <v>71</v>
       </c>
       <c r="O237" t="s">
-        <v>89</v>
+        <v>37</v>
       </c>
       <c r="P237" t="s">
         <v>46</v>
@@ -19365,7 +19365,7 @@
         <v>30</v>
       </c>
       <c r="O242" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P242" t="s">
         <v>97</v>
@@ -19537,7 +19537,7 @@
         <v>56</v>
       </c>
       <c r="W244" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X244" t="s">
         <v>58</v>
@@ -19611,7 +19611,7 @@
         <v>56</v>
       </c>
       <c r="W245" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X245" t="s">
         <v>40</v>
@@ -19661,7 +19661,7 @@
         <v>30</v>
       </c>
       <c r="O246" t="s">
-        <v>89</v>
+        <v>37</v>
       </c>
       <c r="P246" t="s">
         <v>67</v>
@@ -19833,7 +19833,7 @@
         <v>38</v>
       </c>
       <c r="W248" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X248" t="s">
         <v>40</v>
@@ -20129,7 +20129,7 @@
         <v>56</v>
       </c>
       <c r="W252" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X252" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Actualizado dataset con cambios en columnas
</commit_message>
<xml_diff>
--- a/data/dataset_valores.xlsx
+++ b/data/dataset_valores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eriksandoval/Desktop/ZAGAZ/Estaciones/CH4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E01F3CC-1A55-554D-8918-F79D0DD6175B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2047471-AE45-2442-9634-0136D303D656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="760" windowWidth="30160" windowHeight="18880" xr2:uid="{80066C9F-7D8E-B340-8F04-A05F2EBF0A6F}"/>
   </bookViews>
@@ -1478,7 +1478,7 @@
   <dimension ref="A1:X261"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1975,7 +1975,7 @@
         <v>71</v>
       </c>
       <c r="O7" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P7" t="s">
         <v>32</v>
@@ -2049,7 +2049,7 @@
         <v>30</v>
       </c>
       <c r="O8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="P8" t="s">
         <v>32</v>
@@ -2345,7 +2345,7 @@
         <v>30</v>
       </c>
       <c r="O12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="P12" t="s">
         <v>32</v>
@@ -2567,7 +2567,7 @@
         <v>30</v>
       </c>
       <c r="O15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="P15" t="s">
         <v>32</v>
@@ -3603,7 +3603,7 @@
         <v>36</v>
       </c>
       <c r="O29" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P29" t="s">
         <v>32</v>
@@ -4935,7 +4935,7 @@
         <v>36</v>
       </c>
       <c r="O47" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P47" t="s">
         <v>32</v>
@@ -5971,7 +5971,7 @@
         <v>36</v>
       </c>
       <c r="O61" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P61" t="s">
         <v>32</v>
@@ -6489,7 +6489,7 @@
         <v>71</v>
       </c>
       <c r="O68" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P68" t="s">
         <v>32</v>
@@ -7155,7 +7155,7 @@
         <v>36</v>
       </c>
       <c r="O77" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P77" t="s">
         <v>32</v>
@@ -12557,7 +12557,7 @@
         <v>71</v>
       </c>
       <c r="O150" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P150" t="s">
         <v>32</v>
@@ -13963,7 +13963,7 @@
         <v>36</v>
       </c>
       <c r="O169" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P169" t="s">
         <v>32</v>
@@ -14629,7 +14629,7 @@
         <v>36</v>
       </c>
       <c r="O178" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P178" t="s">
         <v>32</v>

</xml_diff>